<commit_message>
Updated the frmaework for the multi prediction and more Streamlit features
</commit_message>
<xml_diff>
--- a/Design.xlsx
+++ b/Design.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/r_fazal_student_tue_nl/Documents/Documents/Masters - Data Science in Engineering/Master Thesis/Replication/GenerativeLSTM/GenerativeLSTM-1.1.0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rehan\OneDrive - TU Eindhoven\Documents\Masters - Data Science in Engineering\Master Thesis\Replication\GenerativeLSTM\GenerativeLSTM-1.1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{435A87D9-C998-49A1-952E-533DF37F212D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0402A2C0-475F-4AC2-B9AC-582FD30DDE98}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39509988-D5AF-448C-9160-90D8F3D2482B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" activeTab="2" xr2:uid="{7C4E9409-2D51-4ACC-B58D-9FFAEF2AA713}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="37470" windowHeight="21840" activeTab="3" xr2:uid="{7C4E9409-2D51-4ACC-B58D-9FFAEF2AA713}"/>
   </bookViews>
   <sheets>
     <sheet name="GenerativeLSTM-1.1.0" sheetId="1" r:id="rId1"/>
     <sheet name="Parameters" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Problem v1" sheetId="2" r:id="rId3"/>
+    <sheet name="Problem v2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Main</t>
   </si>
@@ -44,9 +45,6 @@
   </si>
   <si>
     <t>Model Training</t>
-  </si>
-  <si>
-    <t>predict_next</t>
   </si>
   <si>
     <t>pred_sfx</t>
@@ -157,12 +155,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -819,6 +817,311 @@
         <a:xfrm rot="5400000">
           <a:off x="5705476" y="3538537"/>
           <a:ext cx="962025" cy="1352550"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>295276</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>85726</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Rectangle 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFFEF333-3B80-4B73-83C2-5E816D032E9D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2733676" y="4724400"/>
+          <a:ext cx="1009650" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>log_reader.py</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>190501</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>157163</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Connector: Elbow 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05EC1501-FD76-4D57-AB31-D48621638174}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="2"/>
+          <a:endCxn id="14" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="4555332" y="2416969"/>
+          <a:ext cx="990600" cy="3624262"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 48077"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>390526</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1219200" cy="1986826"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="TextBox 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A1C307B-B6BF-455B-8222-C1E755F95756}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2828926" y="5114924"/>
+          <a:ext cx="1219200" cy="1986826"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Reads csv, xes files and trasform it to respective train and test sets, one_timestamp variable sets only</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> one timestamp for start and end for each activity in the given event</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>103506</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Rectangle 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{081EBCB3-EB36-4408-B748-2B98BC71D0D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12103100" y="5562601"/>
+          <a:ext cx="1600200" cy="255905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>next_event_predictor.py</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>103506</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>518161</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Connector: Elbow 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB85A4B2-49DB-4D1A-98F5-3CB5AD71C061}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="13" idx="2"/>
+          <a:endCxn id="16" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="13089573" y="4722813"/>
+          <a:ext cx="655321" cy="1024255"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -1146,56 +1449,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B16DDD3-E8D2-4CD7-9A7E-7D15C1351B65}">
   <dimension ref="F5:AC30"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="U34" sqref="U34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="6:24" x14ac:dyDescent="0.3">
-      <c r="F5" s="3" t="s">
+    <row r="5" spans="6:24" x14ac:dyDescent="0.25">
+      <c r="F5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
     </row>
-    <row r="15" spans="6:24" x14ac:dyDescent="0.3">
-      <c r="U15" s="3" t="s">
+    <row r="15" spans="6:24" x14ac:dyDescent="0.25">
+      <c r="U15" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="V15" s="3"/>
-      <c r="W15" s="3"/>
-      <c r="X15" s="3"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
     </row>
-    <row r="16" spans="6:24" x14ac:dyDescent="0.3">
-      <c r="K16" s="3" t="s">
+    <row r="16" spans="6:24" x14ac:dyDescent="0.25">
+      <c r="K16" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
     </row>
-    <row r="30" spans="21:29" x14ac:dyDescent="0.3">
-      <c r="U30" s="1" t="s">
+    <row r="30" spans="25:29" x14ac:dyDescent="0.25">
+      <c r="Y30" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Y30" s="1" t="s">
+      <c r="AC30" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="AC30" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1218,22 +1518,22 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>11</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1246,55 +1546,90 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EF445B3-8A66-463C-A50D-9965A7BD6BB1}">
   <dimension ref="A2:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
       <c r="B8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
-      <c r="B10" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA1C7850-0D51-4712-B83F-988253D2567E}">
+  <dimension ref="A2:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>